<commit_message>
organizer and serviceRequest updates
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-PADI-PersonalInterventionRequestPreference.xlsx
+++ b/output/StructureDefinition-PADI-PersonalInterventionRequestPreference.xlsx
@@ -561,7 +561,7 @@
     <t>This element is labeled as a modifier because the intent alters when and how the resource is actually applicable.</t>
   </si>
   <si>
-    <t>proposal</t>
+    <t>directive</t>
   </si>
   <si>
     <t>The kind of service request.</t>
@@ -5311,7 +5311,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" hidden="true">
+    <row r="35">
       <c r="A35" t="s" s="2">
         <v>324</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>43</v>
       </c>
       <c r="G35" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H35" t="s" s="2">
         <v>44</v>
@@ -5651,7 +5651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" hidden="true">
+    <row r="38">
       <c r="A38" t="s" s="2">
         <v>349</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>43</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>44</v>
@@ -5995,7 +5995,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="41" hidden="true">
+    <row r="41">
       <c r="A41" t="s" s="2">
         <v>375</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>43</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>44</v>

</xml_diff>